<commit_message>
Added VSP Test Suite Collection for QA.
</commit_message>
<xml_diff>
--- a/KatalonData/VLinkCCTestData.xlsx
+++ b/KatalonData/VLinkCCTestData.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6509" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6513" uniqueCount="352">
   <si>
     <t>Notes</t>
   </si>
@@ -1091,6 +1091,9 @@
   </si>
   <si>
     <t>Mon Apr 18 13:17:04 EDT 2022</t>
+  </si>
+  <si>
+    <t>Sun Jun 05 22:38:23 EDT 2022</t>
   </si>
 </sst>
 </file>
@@ -1692,7 +1695,7 @@
         <v>149</v>
       </c>
       <c r="B2" t="s">
-        <v>276</v>
+        <v>351</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>267</v>

</xml_diff>

<commit_message>
Added Vlink Auth Test Case and Test Data.
</commit_message>
<xml_diff>
--- a/KatalonData/VLinkCCTestData.xlsx
+++ b/KatalonData/VLinkCCTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD47E7E1-675D-456D-9024-A1B1EEDEC9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C69BF28-B95B-4531-AE3F-3B8FC1805BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8C2F89C9-A10B-4559-913F-0962936A94D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8C2F89C9-A10B-4559-913F-0962936A94D9}"/>
   </bookViews>
   <sheets>
     <sheet name="CCSaleData" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7136" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7036" uniqueCount="298">
   <si>
     <t>Notes</t>
   </si>
@@ -640,45 +640,6 @@
     <t>Unencypted track1 And 2 data FDMS</t>
   </si>
   <si>
-    <t>Mon Apr 18 12:20:55 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Apr 18 12:21:42 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Apr 18 12:22:29 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Apr 18 12:23:16 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Apr 18 12:24:02 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Apr 18 12:24:49 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Apr 18 12:25:36 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Apr 18 12:26:22 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Apr 18 12:27:08 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Apr 18 12:27:55 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Apr 18 12:28:42 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Apr 18 12:29:28 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Apr 18 12:30:14 EDT 2022</t>
-  </si>
-  <si>
     <t>Mon Apr 18 12:31:00 EDT 2022</t>
   </si>
   <si>
@@ -862,9 +823,6 @@
     <t>Mon Apr 18 13:17:04 EDT 2022</t>
   </si>
   <si>
-    <t>Sun Jun 05 22:38:23 EDT 2022</t>
-  </si>
-  <si>
     <t>TSYS CPS</t>
   </si>
   <si>
@@ -893,6 +851,87 @@
   </si>
   <si>
     <t>Vantiv CPS</t>
+  </si>
+  <si>
+    <t>Tue Sep 06 17:22:23 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Sep 06 17:25:13 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Sep 06 17:28:01 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Sep 06 17:30:49 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Sep 06 17:33:38 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Sep 06 17:36:26 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Sep 06 17:39:15 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Sep 06 17:42:03 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Sep 06 17:44:51 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Sep 06 17:47:40 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Sep 06 17:50:28 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Sep 06 17:53:17 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Sep 06 17:56:05 EDT 2022</t>
+  </si>
+  <si>
+    <t>Wed Sep 21 12:09:16 EDT 2022</t>
+  </si>
+  <si>
+    <t>Wed Sep 21 12:12:02 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Sep 23 12:11:17 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Sep 23 12:12:02 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Sep 23 12:12:45 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Sep 23 12:13:27 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Sep 23 12:14:10 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Sep 23 12:14:52 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Sep 23 12:15:34 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Sep 23 12:16:16 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Sep 23 12:16:58 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Sep 23 12:17:40 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Sep 23 12:18:22 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Sep 23 12:19:04 EDT 2022</t>
   </si>
 </sst>
 </file>
@@ -1272,9 +1311,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D907F6-7637-41F5-9F0A-BDDAA86240AA}">
   <dimension ref="A1:AX139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C141" sqref="C141"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V119" sqref="V119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,18 +1529,15 @@
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>274</v>
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>284</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E2" s="1" t="s">
         <v>43</v>
       </c>
@@ -1610,18 +1646,15 @@
       <c r="AX2" s="2"/>
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>200</v>
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" t="s">
+        <v>271</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E3" s="1" t="s">
         <v>43</v>
       </c>
@@ -1677,18 +1710,15 @@
       <c r="AX3" s="2"/>
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>201</v>
+      <c r="A4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>272</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E4" s="1" t="s">
         <v>43</v>
       </c>
@@ -1744,18 +1774,15 @@
       <c r="AX4" s="2"/>
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>202</v>
+      <c r="A5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" t="s">
+        <v>273</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E5" s="1" t="s">
         <v>43</v>
       </c>
@@ -1864,18 +1891,15 @@
       <c r="AX5" s="2"/>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>203</v>
+      <c r="A6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" t="s">
+        <v>274</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E6" s="1" t="s">
         <v>43</v>
       </c>
@@ -1931,18 +1955,15 @@
       <c r="AX6" s="2"/>
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>204</v>
+      <c r="A7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" t="s">
+        <v>275</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E7" s="1" t="s">
         <v>43</v>
       </c>
@@ -1998,18 +2019,15 @@
       <c r="AX7" s="2"/>
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>205</v>
+      <c r="A8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" t="s">
+        <v>276</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E8" s="1" t="s">
         <v>43</v>
       </c>
@@ -2118,18 +2136,15 @@
       <c r="AX8" s="2"/>
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>206</v>
+      <c r="A9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" t="s">
+        <v>277</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E9" s="1" t="s">
         <v>43</v>
       </c>
@@ -2185,18 +2200,15 @@
       <c r="AX9" s="2"/>
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>207</v>
+      <c r="A10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" t="s">
+        <v>278</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E10" s="1" t="s">
         <v>43</v>
       </c>
@@ -2252,18 +2264,15 @@
       <c r="AX10" s="2"/>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>208</v>
+      <c r="A11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" t="s">
+        <v>279</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E11" s="1" t="s">
         <v>43</v>
       </c>
@@ -2372,18 +2381,15 @@
       <c r="AX11" s="2"/>
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>209</v>
+      <c r="A12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B12" t="s">
+        <v>280</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E12" s="1" t="s">
         <v>43</v>
       </c>
@@ -2439,18 +2445,15 @@
       <c r="AX12" s="2"/>
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>210</v>
+      <c r="A13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" t="s">
+        <v>281</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E13" s="1" t="s">
         <v>43</v>
       </c>
@@ -2506,18 +2509,15 @@
       <c r="AX13" s="2"/>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>211</v>
+      <c r="A14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" t="s">
+        <v>282</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E14" s="1" t="s">
         <v>43</v>
       </c>
@@ -2626,17 +2626,14 @@
       <c r="AX14" s="2"/>
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>212</v>
+      <c r="A15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" t="s">
+        <v>283</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>43</v>
@@ -2697,13 +2694,10 @@
         <v>149</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>43</v>
@@ -2764,13 +2758,10 @@
         <v>149</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>43</v>
@@ -2884,13 +2875,10 @@
         <v>149</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>43</v>
@@ -2951,13 +2939,10 @@
         <v>149</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>43</v>
@@ -3018,13 +3003,10 @@
         <v>149</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>43</v>
@@ -3138,13 +3120,10 @@
         <v>149</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>43</v>
@@ -3205,13 +3184,10 @@
         <v>149</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>43</v>
@@ -3272,13 +3248,10 @@
         <v>149</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>43</v>
@@ -3392,13 +3365,10 @@
         <v>149</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>43</v>
@@ -3459,13 +3429,10 @@
         <v>149</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>43</v>
@@ -3526,13 +3493,10 @@
         <v>150</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>43</v>
@@ -3646,13 +3610,10 @@
         <v>149</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>43</v>
@@ -3713,13 +3674,10 @@
         <v>149</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>43</v>
@@ -3780,13 +3738,10 @@
         <v>149</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>43</v>
@@ -3900,13 +3855,10 @@
         <v>149</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>43</v>
@@ -3967,13 +3919,10 @@
         <v>149</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>43</v>
@@ -4034,13 +3983,10 @@
         <v>149</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>43</v>
@@ -4154,13 +4100,10 @@
         <v>149</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>43</v>
@@ -4221,13 +4164,10 @@
         <v>149</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>43</v>
@@ -4288,13 +4228,10 @@
         <v>149</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>43</v>
@@ -4408,13 +4345,10 @@
         <v>149</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>43</v>
@@ -4475,13 +4409,10 @@
         <v>149</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>43</v>
@@ -4544,9 +4475,6 @@
       <c r="B38" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E38" s="1" t="s">
         <v>43</v>
       </c>
@@ -4661,9 +4589,6 @@
       <c r="B39" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E39" s="1" t="s">
         <v>43</v>
       </c>
@@ -4725,9 +4650,6 @@
       <c r="B40" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E40" s="1" t="s">
         <v>43</v>
       </c>
@@ -4789,9 +4711,6 @@
       <c r="B41" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E41" s="1" t="s">
         <v>43</v>
       </c>
@@ -4906,9 +4825,6 @@
       <c r="B42" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E42" s="1" t="s">
         <v>43</v>
       </c>
@@ -4970,9 +4886,6 @@
       <c r="B43" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E43" s="1" t="s">
         <v>43</v>
       </c>
@@ -5034,9 +4947,6 @@
       <c r="B44" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E44" s="1" t="s">
         <v>43</v>
       </c>
@@ -5151,9 +5061,6 @@
       <c r="B45" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E45" s="1" t="s">
         <v>43</v>
       </c>
@@ -5215,9 +5122,6 @@
       <c r="B46" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E46" s="1" t="s">
         <v>43</v>
       </c>
@@ -5279,9 +5183,6 @@
       <c r="B47" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E47" s="1" t="s">
         <v>43</v>
       </c>
@@ -5396,9 +5297,6 @@
       <c r="B48" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E48" s="1" t="s">
         <v>43</v>
       </c>
@@ -5460,9 +5358,6 @@
       <c r="B49" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E49" s="1" t="s">
         <v>43</v>
       </c>
@@ -5522,13 +5417,10 @@
         <v>149</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>43</v>
@@ -5600,13 +5492,10 @@
         <v>149</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>43</v>
@@ -5731,13 +5620,10 @@
         <v>149</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>43</v>
@@ -5809,13 +5695,10 @@
         <v>149</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>43</v>
@@ -5940,13 +5823,10 @@
         <v>150</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>43</v>
@@ -6018,13 +5898,10 @@
         <v>149</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>43</v>
@@ -6149,13 +6026,10 @@
         <v>149</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>43</v>
@@ -6227,13 +6101,10 @@
         <v>149</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>43</v>
@@ -6358,13 +6229,10 @@
         <v>150</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>43</v>
@@ -6436,13 +6304,10 @@
         <v>149</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>43</v>
@@ -6567,13 +6432,10 @@
         <v>149</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>43</v>
@@ -6645,13 +6507,10 @@
         <v>149</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>43</v>
@@ -6781,9 +6640,6 @@
       <c r="C62" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E62" s="1" t="s">
         <v>43</v>
       </c>
@@ -6912,9 +6768,6 @@
       <c r="C63" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E63" s="1" t="s">
         <v>43</v>
       </c>
@@ -6990,9 +6843,6 @@
       <c r="C64" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E64" s="1" t="s">
         <v>43</v>
       </c>
@@ -7068,9 +6918,6 @@
       <c r="C65" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E65" s="1" t="s">
         <v>43</v>
       </c>
@@ -7199,9 +7046,6 @@
       <c r="C66" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E66" s="1" t="s">
         <v>43</v>
       </c>
@@ -7277,9 +7121,6 @@
       <c r="C67" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E67" s="1" t="s">
         <v>43</v>
       </c>
@@ -7355,9 +7196,6 @@
       <c r="C68" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E68" s="1" t="s">
         <v>43</v>
       </c>
@@ -7486,9 +7324,6 @@
       <c r="C69" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E69" s="1" t="s">
         <v>43</v>
       </c>
@@ -7564,9 +7399,6 @@
       <c r="C70" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E70" s="1" t="s">
         <v>43</v>
       </c>
@@ -7642,9 +7474,6 @@
       <c r="C71" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E71" s="1" t="s">
         <v>43</v>
       </c>
@@ -7773,9 +7602,6 @@
       <c r="C72" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D72" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E72" s="1" t="s">
         <v>43</v>
       </c>
@@ -7851,9 +7677,6 @@
       <c r="C73" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E73" s="1" t="s">
         <v>43</v>
       </c>
@@ -7924,13 +7747,10 @@
         <v>149</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>43</v>
@@ -8002,13 +7822,10 @@
         <v>149</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>43</v>
@@ -8133,13 +7950,10 @@
         <v>149</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>43</v>
@@ -8211,13 +8025,10 @@
         <v>149</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>43</v>
@@ -8342,13 +8153,10 @@
         <v>150</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>43</v>
@@ -8420,13 +8228,10 @@
         <v>149</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>43</v>
@@ -8551,13 +8356,10 @@
         <v>149</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>43</v>
@@ -8629,13 +8431,10 @@
         <v>149</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>43</v>
@@ -8760,13 +8559,10 @@
         <v>150</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>43</v>
@@ -8838,13 +8634,10 @@
         <v>149</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>43</v>
@@ -8969,13 +8762,10 @@
         <v>149</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>43</v>
@@ -9047,13 +8837,10 @@
         <v>149</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>43</v>
@@ -9183,9 +8970,6 @@
       <c r="C86" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D86" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E86" s="1" t="s">
         <v>43</v>
       </c>
@@ -9314,9 +9098,6 @@
       <c r="C87" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D87" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E87" s="1" t="s">
         <v>43</v>
       </c>
@@ -9392,9 +9173,6 @@
       <c r="C88" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E88" s="1" t="s">
         <v>43</v>
       </c>
@@ -9470,9 +9248,6 @@
       <c r="C89" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D89" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E89" s="1" t="s">
         <v>43</v>
       </c>
@@ -9601,9 +9376,6 @@
       <c r="C90" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D90" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E90" s="1" t="s">
         <v>43</v>
       </c>
@@ -9679,9 +9451,6 @@
       <c r="C91" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D91" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E91" s="1" t="s">
         <v>43</v>
       </c>
@@ -9757,9 +9526,6 @@
       <c r="C92" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D92" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E92" s="1" t="s">
         <v>43</v>
       </c>
@@ -9888,9 +9654,6 @@
       <c r="C93" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D93" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E93" s="1" t="s">
         <v>43</v>
       </c>
@@ -9966,9 +9729,6 @@
       <c r="C94" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D94" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E94" s="1" t="s">
         <v>43</v>
       </c>
@@ -10044,9 +9804,6 @@
       <c r="C95" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D95" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E95" s="1" t="s">
         <v>43</v>
       </c>
@@ -10175,9 +9932,6 @@
       <c r="C96" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D96" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E96" s="1" t="s">
         <v>43</v>
       </c>
@@ -10253,9 +10007,6 @@
       <c r="C97" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D97" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E97" s="1" t="s">
         <v>43</v>
       </c>
@@ -10326,13 +10077,10 @@
         <v>150</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>43</v>
@@ -10384,13 +10132,10 @@
         <v>149</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>43</v>
@@ -10442,13 +10187,10 @@
         <v>149</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>43</v>
@@ -10505,9 +10247,6 @@
       <c r="C101" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D101" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E101" s="1" t="s">
         <v>43</v>
       </c>
@@ -10563,9 +10302,6 @@
       <c r="C102" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D102" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E102" s="1" t="s">
         <v>43</v>
       </c>
@@ -10621,9 +10357,6 @@
       <c r="C103" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D103" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E103" s="1" t="s">
         <v>43</v>
       </c>
@@ -10674,13 +10407,10 @@
         <v>149</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>43</v>
@@ -10717,13 +10447,10 @@
         <v>150</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>43</v>
@@ -10760,13 +10487,10 @@
         <v>149</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>43</v>
@@ -10806,13 +10530,10 @@
         <v>149</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>43</v>
@@ -10852,13 +10573,10 @@
         <v>149</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>43</v>
@@ -10895,13 +10613,10 @@
         <v>150</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>43</v>
@@ -10938,13 +10653,10 @@
         <v>149</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>43</v>
@@ -10984,13 +10696,10 @@
         <v>149</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>43</v>
@@ -11030,13 +10739,10 @@
         <v>149</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>43</v>
@@ -11073,13 +10779,10 @@
         <v>150</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>43</v>
@@ -11116,13 +10819,10 @@
         <v>149</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>43</v>
@@ -11162,14 +10862,11 @@
         <v>149</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="D115" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E115" s="1" t="s">
         <v>43</v>
       </c>
@@ -11204,10 +10901,14 @@
       <c r="AX115" s="2"/>
     </row>
     <row r="116" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A116" s="3"/>
-      <c r="B116" s="3"/>
+      <c r="A116" t="s">
+        <v>149</v>
+      </c>
+      <c r="B116" t="s">
+        <v>286</v>
+      </c>
       <c r="C116" s="1" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>188</v>
@@ -11219,7 +10920,7 @@
         <v>44</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="H116" s="1" t="s">
         <v>45</v>
@@ -11258,7 +10959,7 @@
         <v>54</v>
       </c>
       <c r="V116" s="1" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="W116" s="1" t="s">
         <v>102</v>
@@ -11320,10 +11021,14 @@
       <c r="AX116" s="2"/>
     </row>
     <row r="117" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A117" s="3"/>
-      <c r="B117" s="3"/>
+      <c r="A117" t="s">
+        <v>149</v>
+      </c>
+      <c r="B117" t="s">
+        <v>287</v>
+      </c>
       <c r="C117" s="1" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>188</v>
@@ -11335,7 +11040,7 @@
         <v>44</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="H117" s="1" t="s">
         <v>45</v>
@@ -11374,7 +11079,7 @@
         <v>54</v>
       </c>
       <c r="V117" s="1" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="W117" s="1" t="s">
         <v>102</v>
@@ -11436,10 +11141,14 @@
       <c r="AX117" s="2"/>
     </row>
     <row r="118" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A118" s="3"/>
-      <c r="B118" s="3"/>
+      <c r="A118" t="s">
+        <v>149</v>
+      </c>
+      <c r="B118" t="s">
+        <v>288</v>
+      </c>
       <c r="C118" s="1" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>188</v>
@@ -11451,7 +11160,7 @@
         <v>44</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="H118" s="1" t="s">
         <v>45</v>
@@ -11490,7 +11199,7 @@
         <v>54</v>
       </c>
       <c r="V118" s="1" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="W118" s="1" t="s">
         <v>102</v>
@@ -11552,10 +11261,14 @@
       <c r="AX118" s="2"/>
     </row>
     <row r="119" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A119" s="3"/>
-      <c r="B119" s="3"/>
+      <c r="A119" t="s">
+        <v>149</v>
+      </c>
+      <c r="B119" t="s">
+        <v>289</v>
+      </c>
       <c r="C119" s="1" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>188</v>
@@ -11567,7 +11280,7 @@
         <v>44</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="H119" s="1" t="s">
         <v>45</v>
@@ -11606,7 +11319,7 @@
         <v>54</v>
       </c>
       <c r="V119" s="1" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="W119" s="1" t="s">
         <v>102</v>
@@ -11668,10 +11381,14 @@
       <c r="AX119" s="2"/>
     </row>
     <row r="120" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A120" s="3"/>
-      <c r="B120" s="3"/>
+      <c r="A120" t="s">
+        <v>149</v>
+      </c>
+      <c r="B120" t="s">
+        <v>290</v>
+      </c>
       <c r="C120" s="1" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>188</v>
@@ -11683,7 +11400,7 @@
         <v>44</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="H120" s="1" t="s">
         <v>45</v>
@@ -11722,7 +11439,7 @@
         <v>54</v>
       </c>
       <c r="V120" s="1" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="W120" s="1" t="s">
         <v>102</v>
@@ -11784,10 +11501,14 @@
       <c r="AX120" s="2"/>
     </row>
     <row r="121" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A121" s="3"/>
-      <c r="B121" s="3"/>
+      <c r="A121" t="s">
+        <v>149</v>
+      </c>
+      <c r="B121" t="s">
+        <v>291</v>
+      </c>
       <c r="C121" s="1" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>188</v>
@@ -11799,7 +11520,7 @@
         <v>44</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="H121" s="1" t="s">
         <v>45</v>
@@ -11838,7 +11559,7 @@
         <v>54</v>
       </c>
       <c r="V121" s="1" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="W121" s="1" t="s">
         <v>102</v>
@@ -11900,10 +11621,14 @@
       <c r="AX121" s="2"/>
     </row>
     <row r="122" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A122" s="3"/>
-      <c r="B122" s="3"/>
+      <c r="A122" t="s">
+        <v>149</v>
+      </c>
+      <c r="B122" t="s">
+        <v>292</v>
+      </c>
       <c r="C122" s="1" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>188</v>
@@ -11915,7 +11640,7 @@
         <v>44</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="H122" s="1" t="s">
         <v>45</v>
@@ -11954,7 +11679,7 @@
         <v>54</v>
       </c>
       <c r="V122" s="1" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="W122" s="1" t="s">
         <v>102</v>
@@ -12016,10 +11741,14 @@
       <c r="AX122" s="2"/>
     </row>
     <row r="123" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A123" s="3"/>
-      <c r="B123" s="3"/>
+      <c r="A123" t="s">
+        <v>149</v>
+      </c>
+      <c r="B123" t="s">
+        <v>293</v>
+      </c>
       <c r="C123" s="1" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>188</v>
@@ -12031,7 +11760,7 @@
         <v>44</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="H123" s="1" t="s">
         <v>45</v>
@@ -12070,7 +11799,7 @@
         <v>54</v>
       </c>
       <c r="V123" s="1" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="W123" s="1" t="s">
         <v>102</v>
@@ -12132,10 +11861,14 @@
       <c r="AX123" s="2"/>
     </row>
     <row r="124" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A124" s="3"/>
-      <c r="B124" s="3"/>
+      <c r="A124" t="s">
+        <v>149</v>
+      </c>
+      <c r="B124" t="s">
+        <v>294</v>
+      </c>
       <c r="C124" s="1" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>188</v>
@@ -12147,7 +11880,7 @@
         <v>44</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="H124" s="1" t="s">
         <v>45</v>
@@ -12186,7 +11919,7 @@
         <v>54</v>
       </c>
       <c r="V124" s="1" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="W124" s="1" t="s">
         <v>102</v>
@@ -12248,10 +11981,14 @@
       <c r="AX124" s="2"/>
     </row>
     <row r="125" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A125" s="3"/>
-      <c r="B125" s="3"/>
+      <c r="A125" t="s">
+        <v>149</v>
+      </c>
+      <c r="B125" t="s">
+        <v>295</v>
+      </c>
       <c r="C125" s="1" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>188</v>
@@ -12263,7 +12000,7 @@
         <v>44</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="H125" s="1" t="s">
         <v>45</v>
@@ -12302,7 +12039,7 @@
         <v>54</v>
       </c>
       <c r="V125" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="W125" s="1" t="s">
         <v>102</v>
@@ -12364,10 +12101,14 @@
       <c r="AX125" s="2"/>
     </row>
     <row r="126" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A126" s="3"/>
-      <c r="B126" s="3"/>
+      <c r="A126" t="s">
+        <v>149</v>
+      </c>
+      <c r="B126" t="s">
+        <v>296</v>
+      </c>
       <c r="C126" s="1" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>188</v>
@@ -12379,7 +12120,7 @@
         <v>44</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="H126" s="1" t="s">
         <v>45</v>
@@ -12418,7 +12159,7 @@
         <v>54</v>
       </c>
       <c r="V126" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="W126" s="1" t="s">
         <v>102</v>
@@ -12480,10 +12221,14 @@
       <c r="AX126" s="2"/>
     </row>
     <row r="127" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A127" s="3"/>
-      <c r="B127" s="3"/>
+      <c r="A127" t="s">
+        <v>149</v>
+      </c>
+      <c r="B127" t="s">
+        <v>297</v>
+      </c>
       <c r="C127" s="1" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>188</v>
@@ -12495,7 +12240,7 @@
         <v>44</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="H127" s="1" t="s">
         <v>45</v>
@@ -12534,7 +12279,7 @@
         <v>54</v>
       </c>
       <c r="V127" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="W127" s="1" t="s">
         <v>102</v>
@@ -12596,13 +12341,14 @@
       <c r="AX127" s="2"/>
     </row>
     <row r="128" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A128" s="3"/>
-      <c r="B128" s="3"/>
+      <c r="A128" t="s">
+        <v>149</v>
+      </c>
+      <c r="B128" t="s">
+        <v>285</v>
+      </c>
       <c r="C128" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>188</v>
+        <v>270</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>43</v>
@@ -12611,13 +12357,13 @@
         <v>44</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="J128" s="1" t="s">
         <v>47</v>
@@ -12650,7 +12396,7 @@
         <v>54</v>
       </c>
       <c r="V128" s="1" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="W128" s="1" t="s">
         <v>102</v>
@@ -12715,10 +12461,7 @@
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>188</v>
+        <v>270</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>43</v>
@@ -12727,13 +12470,13 @@
         <v>44</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="J129" s="1" t="s">
         <v>47</v>
@@ -12766,7 +12509,7 @@
         <v>54</v>
       </c>
       <c r="V129" s="1" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="W129" s="1" t="s">
         <v>102</v>
@@ -12831,10 +12574,7 @@
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>188</v>
+        <v>270</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>43</v>
@@ -12843,13 +12583,13 @@
         <v>44</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="H130" s="1" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="J130" s="1" t="s">
         <v>47</v>
@@ -12882,7 +12622,7 @@
         <v>54</v>
       </c>
       <c r="V130" s="1" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="W130" s="1" t="s">
         <v>102</v>
@@ -12947,10 +12687,7 @@
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>188</v>
+        <v>270</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>43</v>
@@ -12959,13 +12696,13 @@
         <v>44</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="H131" s="1" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="J131" s="1" t="s">
         <v>47</v>
@@ -12998,7 +12735,7 @@
         <v>54</v>
       </c>
       <c r="V131" s="1" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="W131" s="1" t="s">
         <v>102</v>
@@ -13063,10 +12800,7 @@
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>188</v>
+        <v>270</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>43</v>
@@ -13075,13 +12809,13 @@
         <v>44</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="J132" s="1" t="s">
         <v>47</v>
@@ -13114,7 +12848,7 @@
         <v>54</v>
       </c>
       <c r="V132" s="1" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="W132" s="1" t="s">
         <v>102</v>
@@ -13179,10 +12913,7 @@
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>188</v>
+        <v>270</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>43</v>
@@ -13191,13 +12922,13 @@
         <v>44</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="J133" s="1" t="s">
         <v>47</v>
@@ -13230,7 +12961,7 @@
         <v>54</v>
       </c>
       <c r="V133" s="1" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="W133" s="1" t="s">
         <v>102</v>
@@ -13295,10 +13026,7 @@
       <c r="A134" s="3"/>
       <c r="B134" s="3"/>
       <c r="C134" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>188</v>
+        <v>270</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>43</v>
@@ -13307,13 +13035,13 @@
         <v>44</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="H134" s="1" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="J134" s="1" t="s">
         <v>47</v>
@@ -13346,7 +13074,7 @@
         <v>54</v>
       </c>
       <c r="V134" s="1" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="W134" s="1" t="s">
         <v>102</v>
@@ -13411,10 +13139,7 @@
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
       <c r="C135" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>188</v>
+        <v>270</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>43</v>
@@ -13423,13 +13148,13 @@
         <v>44</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="H135" s="1" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="J135" s="1" t="s">
         <v>47</v>
@@ -13462,7 +13187,7 @@
         <v>54</v>
       </c>
       <c r="V135" s="1" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="W135" s="1" t="s">
         <v>102</v>
@@ -13527,10 +13252,7 @@
       <c r="A136" s="3"/>
       <c r="B136" s="3"/>
       <c r="C136" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>188</v>
+        <v>270</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>43</v>
@@ -13539,13 +13261,13 @@
         <v>44</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="J136" s="1" t="s">
         <v>47</v>
@@ -13578,7 +13300,7 @@
         <v>54</v>
       </c>
       <c r="V136" s="1" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="W136" s="1" t="s">
         <v>102</v>
@@ -13643,10 +13365,7 @@
       <c r="A137" s="3"/>
       <c r="B137" s="3"/>
       <c r="C137" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>188</v>
+        <v>270</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>43</v>
@@ -13655,13 +13374,13 @@
         <v>44</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="J137" s="1" t="s">
         <v>47</v>
@@ -13694,7 +13413,7 @@
         <v>54</v>
       </c>
       <c r="V137" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="W137" s="1" t="s">
         <v>102</v>
@@ -13759,10 +13478,7 @@
       <c r="A138" s="3"/>
       <c r="B138" s="3"/>
       <c r="C138" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>188</v>
+        <v>270</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>43</v>
@@ -13771,13 +13487,13 @@
         <v>44</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="H138" s="1" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="J138" s="1" t="s">
         <v>47</v>
@@ -13810,7 +13526,7 @@
         <v>54</v>
       </c>
       <c r="V138" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="W138" s="1" t="s">
         <v>102</v>
@@ -13875,10 +13591,7 @@
       <c r="A139" s="3"/>
       <c r="B139" s="3"/>
       <c r="C139" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>188</v>
+        <v>270</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>43</v>
@@ -13887,13 +13600,13 @@
         <v>44</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="H139" s="1" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="J139" s="1" t="s">
         <v>47</v>
@@ -13926,7 +13639,7 @@
         <v>54</v>
       </c>
       <c r="V139" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="W139" s="1" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
Updated VLink Test Cases to include Demo2 Profile.
</commit_message>
<xml_diff>
--- a/KatalonData/VLinkCCTestData.xlsx
+++ b/KatalonData/VLinkCCTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5740408-2ECA-41F2-9329-9D38436D52DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B23CCB-F526-438A-8882-3C8FE958A62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8C2F89C9-A10B-4559-913F-0962936A94D9}"/>
+    <workbookView xWindow="-18825" yWindow="1950" windowWidth="15435" windowHeight="11970" xr2:uid="{8C2F89C9-A10B-4559-913F-0962936A94D9}"/>
   </bookViews>
   <sheets>
     <sheet name="CCSaleData" sheetId="1" r:id="rId1"/>
@@ -1344,7 +1344,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D907F6-7637-41F5-9F0A-BDDAA86240AA}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AX139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1684,7 +1683,7 @@
       </c>
       <c r="AX2" s="2"/>
     </row>
-    <row r="3" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>149</v>
       </c>
@@ -1751,7 +1750,7 @@
       <c r="AE3" s="2"/>
       <c r="AX3" s="2"/>
     </row>
-    <row r="4" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -1938,7 +1937,7 @@
       </c>
       <c r="AX5" s="2"/>
     </row>
-    <row r="6" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>149</v>
       </c>
@@ -2005,7 +2004,7 @@
       <c r="AE6" s="2"/>
       <c r="AX6" s="2"/>
     </row>
-    <row r="7" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>149</v>
       </c>
@@ -2192,7 +2191,7 @@
       </c>
       <c r="AX8" s="2"/>
     </row>
-    <row r="9" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>149</v>
       </c>
@@ -2259,7 +2258,7 @@
       <c r="AE9" s="2"/>
       <c r="AX9" s="2"/>
     </row>
-    <row r="10" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>149</v>
       </c>
@@ -2446,7 +2445,7 @@
       </c>
       <c r="AX11" s="2"/>
     </row>
-    <row r="12" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>149</v>
       </c>
@@ -2513,7 +2512,7 @@
       <c r="AE12" s="2"/>
       <c r="AX12" s="2"/>
     </row>
-    <row r="13" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>149</v>
       </c>
@@ -2700,7 +2699,7 @@
       </c>
       <c r="AX14" s="2"/>
     </row>
-    <row r="15" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>149</v>
       </c>
@@ -2767,7 +2766,7 @@
       <c r="AE15" s="2"/>
       <c r="AX15" s="2"/>
     </row>
-    <row r="16" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>149</v>
       </c>
@@ -2954,7 +2953,7 @@
       </c>
       <c r="AX17" s="2"/>
     </row>
-    <row r="18" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>149</v>
       </c>
@@ -3021,7 +3020,7 @@
       <c r="AE18" s="2"/>
       <c r="AX18" s="2"/>
     </row>
-    <row r="19" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>149</v>
       </c>
@@ -3208,7 +3207,7 @@
       </c>
       <c r="AX20" s="2"/>
     </row>
-    <row r="21" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>149</v>
       </c>
@@ -3275,7 +3274,7 @@
       <c r="AE21" s="2"/>
       <c r="AX21" s="2"/>
     </row>
-    <row r="22" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>149</v>
       </c>
@@ -3462,7 +3461,7 @@
       </c>
       <c r="AX23" s="2"/>
     </row>
-    <row r="24" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>149</v>
       </c>
@@ -3529,7 +3528,7 @@
       <c r="AE24" s="2"/>
       <c r="AX24" s="2"/>
     </row>
-    <row r="25" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>149</v>
       </c>
@@ -3716,7 +3715,7 @@
       </c>
       <c r="AX26" s="2"/>
     </row>
-    <row r="27" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>149</v>
       </c>
@@ -3783,7 +3782,7 @@
       <c r="AE27" s="2"/>
       <c r="AX27" s="2"/>
     </row>
-    <row r="28" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>149</v>
       </c>
@@ -3970,7 +3969,7 @@
       </c>
       <c r="AX29" s="2"/>
     </row>
-    <row r="30" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>149</v>
       </c>
@@ -4037,7 +4036,7 @@
       <c r="AE30" s="2"/>
       <c r="AX30" s="2"/>
     </row>
-    <row r="31" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>149</v>
       </c>
@@ -4224,7 +4223,7 @@
       </c>
       <c r="AX32" s="2"/>
     </row>
-    <row r="33" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>149</v>
       </c>
@@ -4291,7 +4290,7 @@
       <c r="AE33" s="2"/>
       <c r="AX33" s="2"/>
     </row>
-    <row r="34" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>149</v>
       </c>
@@ -4478,7 +4477,7 @@
       </c>
       <c r="AX35" s="2"/>
     </row>
-    <row r="36" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>149</v>
       </c>
@@ -4545,7 +4544,7 @@
       <c r="AE36" s="2"/>
       <c r="AX36" s="2"/>
     </row>
-    <row r="37" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -4612,7 +4611,7 @@
       <c r="AE37" s="2"/>
       <c r="AX37" s="2"/>
     </row>
-    <row r="38" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -4729,7 +4728,7 @@
       </c>
       <c r="AX38" s="2"/>
     </row>
-    <row r="39" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>149</v>
       </c>
@@ -4793,7 +4792,7 @@
       <c r="AE39" s="2"/>
       <c r="AX39" s="2"/>
     </row>
-    <row r="40" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -4857,7 +4856,7 @@
       <c r="AE40" s="2"/>
       <c r="AX40" s="2"/>
     </row>
-    <row r="41" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>149</v>
       </c>
@@ -4974,7 +4973,7 @@
       </c>
       <c r="AX41" s="2"/>
     </row>
-    <row r="42" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>149</v>
       </c>
@@ -5038,7 +5037,7 @@
       <c r="AE42" s="2"/>
       <c r="AX42" s="2"/>
     </row>
-    <row r="43" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>149</v>
       </c>
@@ -5102,7 +5101,7 @@
       <c r="AE43" s="2"/>
       <c r="AX43" s="2"/>
     </row>
-    <row r="44" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>149</v>
       </c>
@@ -5219,7 +5218,7 @@
       </c>
       <c r="AX44" s="2"/>
     </row>
-    <row r="45" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>149</v>
       </c>
@@ -5283,7 +5282,7 @@
       <c r="AE45" s="2"/>
       <c r="AX45" s="2"/>
     </row>
-    <row r="46" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>149</v>
       </c>
@@ -5347,7 +5346,7 @@
       <c r="AE46" s="2"/>
       <c r="AX46" s="2"/>
     </row>
-    <row r="47" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>149</v>
       </c>
@@ -5464,7 +5463,7 @@
       </c>
       <c r="AX47" s="2"/>
     </row>
-    <row r="48" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>149</v>
       </c>
@@ -5528,7 +5527,7 @@
       <c r="AE48" s="2"/>
       <c r="AX48" s="2"/>
     </row>
-    <row r="49" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>149</v>
       </c>
@@ -6846,7 +6845,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="62" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>150</v>
       </c>
@@ -6977,7 +6976,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="63" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>149</v>
       </c>
@@ -7055,7 +7054,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="64" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>149</v>
       </c>
@@ -7133,7 +7132,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="65" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>149</v>
       </c>
@@ -7264,7 +7263,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="66" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>149</v>
       </c>
@@ -7342,7 +7341,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>149</v>
       </c>
@@ -7420,7 +7419,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="68" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>149</v>
       </c>
@@ -7551,7 +7550,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>149</v>
       </c>
@@ -7629,7 +7628,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="70" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>149</v>
       </c>
@@ -7707,7 +7706,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>149</v>
       </c>
@@ -7838,7 +7837,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="72" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>149</v>
       </c>
@@ -7916,7 +7915,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="73" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>149</v>
       </c>
@@ -9248,7 +9247,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="86" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>150</v>
       </c>
@@ -9379,7 +9378,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="87" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>149</v>
       </c>
@@ -9457,7 +9456,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="88" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>149</v>
       </c>
@@ -9535,7 +9534,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="89" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>149</v>
       </c>
@@ -9666,7 +9665,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="90" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>149</v>
       </c>
@@ -9744,7 +9743,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="91" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>149</v>
       </c>
@@ -9822,7 +9821,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="92" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>149</v>
       </c>
@@ -9953,7 +9952,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="93" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>149</v>
       </c>
@@ -10031,7 +10030,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="94" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>149</v>
       </c>
@@ -10109,7 +10108,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="95" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>149</v>
       </c>
@@ -10240,7 +10239,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="96" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>149</v>
       </c>
@@ -10318,7 +10317,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="97" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>149</v>
       </c>
@@ -10570,7 +10569,7 @@
       <c r="AE100" s="2"/>
       <c r="AX100" s="2"/>
     </row>
-    <row r="101" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>149</v>
       </c>
@@ -10628,7 +10627,7 @@
       <c r="AE101" s="2"/>
       <c r="AX101" s="2"/>
     </row>
-    <row r="102" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>149</v>
       </c>
@@ -10686,7 +10685,7 @@
       <c r="AE102" s="2"/>
       <c r="AX102" s="2"/>
     </row>
-    <row r="103" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>149</v>
       </c>
@@ -10922,7 +10921,7 @@
       <c r="AE107" s="2"/>
       <c r="AX107" s="2"/>
     </row>
-    <row r="108" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>149</v>
       </c>
@@ -10965,7 +10964,7 @@
       <c r="AE108" s="2"/>
       <c r="AX108" s="2"/>
     </row>
-    <row r="109" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>150</v>
       </c>
@@ -11008,7 +11007,7 @@
       <c r="AE109" s="2"/>
       <c r="AX109" s="2"/>
     </row>
-    <row r="110" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>149</v>
       </c>
@@ -11054,7 +11053,7 @@
       <c r="AE110" s="2"/>
       <c r="AX110" s="2"/>
     </row>
-    <row r="111" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>149</v>
       </c>
@@ -11100,7 +11099,7 @@
       <c r="AE111" s="2"/>
       <c r="AX111" s="2"/>
     </row>
-    <row r="112" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>149</v>
       </c>
@@ -11143,7 +11142,7 @@
       <c r="AE112" s="2"/>
       <c r="AX112" s="2"/>
     </row>
-    <row r="113" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>150</v>
       </c>
@@ -11186,7 +11185,7 @@
       <c r="AE113" s="2"/>
       <c r="AX113" s="2"/>
     </row>
-    <row r="114" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>149</v>
       </c>
@@ -11232,7 +11231,7 @@
       <c r="AE114" s="2"/>
       <c r="AX114" s="2"/>
     </row>
-    <row r="115" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>149</v>
       </c>
@@ -11278,7 +11277,7 @@
       <c r="AE115" s="2"/>
       <c r="AX115" s="2"/>
     </row>
-    <row r="116" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>149</v>
       </c>
@@ -11398,7 +11397,7 @@
       </c>
       <c r="AX116" s="2"/>
     </row>
-    <row r="117" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>149</v>
       </c>
@@ -11518,7 +11517,7 @@
       </c>
       <c r="AX117" s="2"/>
     </row>
-    <row r="118" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>149</v>
       </c>
@@ -11638,7 +11637,7 @@
       </c>
       <c r="AX118" s="2"/>
     </row>
-    <row r="119" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>149</v>
       </c>
@@ -11758,7 +11757,7 @@
       </c>
       <c r="AX119" s="2"/>
     </row>
-    <row r="120" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>149</v>
       </c>
@@ -11878,7 +11877,7 @@
       </c>
       <c r="AX120" s="2"/>
     </row>
-    <row r="121" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>149</v>
       </c>
@@ -11998,7 +11997,7 @@
       </c>
       <c r="AX121" s="2"/>
     </row>
-    <row r="122" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>149</v>
       </c>
@@ -12118,7 +12117,7 @@
       </c>
       <c r="AX122" s="2"/>
     </row>
-    <row r="123" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>149</v>
       </c>
@@ -12238,7 +12237,7 @@
       </c>
       <c r="AX123" s="2"/>
     </row>
-    <row r="124" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>149</v>
       </c>
@@ -12358,7 +12357,7 @@
       </c>
       <c r="AX124" s="2"/>
     </row>
-    <row r="125" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>149</v>
       </c>
@@ -12478,7 +12477,7 @@
       </c>
       <c r="AX125" s="2"/>
     </row>
-    <row r="126" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>149</v>
       </c>
@@ -12598,7 +12597,7 @@
       </c>
       <c r="AX126" s="2"/>
     </row>
-    <row r="127" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>149</v>
       </c>
@@ -12718,7 +12717,7 @@
       </c>
       <c r="AX127" s="2"/>
     </row>
-    <row r="128" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>149</v>
       </c>
@@ -12838,7 +12837,7 @@
       </c>
       <c r="AX128" s="2"/>
     </row>
-    <row r="129" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>149</v>
       </c>
@@ -12958,7 +12957,7 @@
       </c>
       <c r="AX129" s="2"/>
     </row>
-    <row r="130" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>149</v>
       </c>
@@ -13078,7 +13077,7 @@
       </c>
       <c r="AX130" s="2"/>
     </row>
-    <row r="131" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>149</v>
       </c>
@@ -13198,7 +13197,7 @@
       </c>
       <c r="AX131" s="2"/>
     </row>
-    <row r="132" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>149</v>
       </c>
@@ -13318,7 +13317,7 @@
       </c>
       <c r="AX132" s="2"/>
     </row>
-    <row r="133" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>149</v>
       </c>
@@ -13438,7 +13437,7 @@
       </c>
       <c r="AX133" s="2"/>
     </row>
-    <row r="134" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>149</v>
       </c>
@@ -13558,7 +13557,7 @@
       </c>
       <c r="AX134" s="2"/>
     </row>
-    <row r="135" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>149</v>
       </c>
@@ -13678,7 +13677,7 @@
       </c>
       <c r="AX135" s="2"/>
     </row>
-    <row r="136" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>149</v>
       </c>
@@ -13798,7 +13797,7 @@
       </c>
       <c r="AX136" s="2"/>
     </row>
-    <row r="137" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>149</v>
       </c>
@@ -13918,7 +13917,7 @@
       </c>
       <c r="AX137" s="2"/>
     </row>
-    <row r="138" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>149</v>
       </c>
@@ -14038,7 +14037,7 @@
       </c>
       <c r="AX138" s="2"/>
     </row>
-    <row r="139" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>149</v>
       </c>
@@ -14159,13 +14158,7 @@
       <c r="AX139" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="G1:G139" xr:uid="{01D907F6-7637-41F5-9F0A-BDDAA86240AA}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="665"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="G1:G139" xr:uid="{01D907F6-7637-41F5-9F0A-BDDAA86240AA}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated test data for Unencrypted track data.
</commit_message>
<xml_diff>
--- a/KatalonData/VLinkCCTestData.xlsx
+++ b/KatalonData/VLinkCCTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B23CCB-F526-438A-8882-3C8FE958A62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA55319-69FB-42A0-B0D8-134DB0D4D809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18825" yWindow="1950" windowWidth="15435" windowHeight="11970" xr2:uid="{8C2F89C9-A10B-4559-913F-0962936A94D9}"/>
+    <workbookView xWindow="4740" yWindow="615" windowWidth="17010" windowHeight="13935" xr2:uid="{8C2F89C9-A10B-4559-913F-0962936A94D9}"/>
   </bookViews>
   <sheets>
     <sheet name="CCSaleData" sheetId="1" r:id="rId1"/>
@@ -1346,9 +1346,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D907F6-7637-41F5-9F0A-BDDAA86240AA}">
   <dimension ref="A1:AX139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA104" sqref="AA104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated TestVRelayLiveDeployments Script to add new Excel spreadsheet provided by Thilys.
</commit_message>
<xml_diff>
--- a/KatalonData/VLinkCCTestData.xlsx
+++ b/KatalonData/VLinkCCTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA55319-69FB-42A0-B0D8-134DB0D4D809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0FEF0F-93B4-419F-A7B2-AC48DF9E8886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="615" windowWidth="17010" windowHeight="13935" xr2:uid="{8C2F89C9-A10B-4559-913F-0962936A94D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8C2F89C9-A10B-4559-913F-0962936A94D9}"/>
   </bookViews>
   <sheets>
     <sheet name="CCSaleData" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7184" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7184" uniqueCount="313">
   <si>
     <t>Notes</t>
   </si>
@@ -968,6 +968,15 @@
   </si>
   <si>
     <t>Do not Execute Fails</t>
+  </si>
+  <si>
+    <t>%B5567080011582687^AHMED/IMTIAZ              ^2603201090300000000000528000015?;5567080011582687=26032010903052800015?</t>
+  </si>
+  <si>
+    <t>%B5567080011582687^AHMED/IMTIAZ              ^2603201090300000000000528000015?</t>
+  </si>
+  <si>
+    <t>;5567080011582687=26032010903052800015?</t>
   </si>
 </sst>
 </file>
@@ -1347,8 +1356,8 @@
   <dimension ref="A1:AX139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA104" sqref="AA104"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA117" sqref="AA117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10781,7 +10790,7 @@
         <v>54</v>
       </c>
       <c r="AA104" s="1" t="s">
-        <v>141</v>
+        <v>310</v>
       </c>
       <c r="AE104" s="2"/>
       <c r="AX104" s="2"/>
@@ -10824,7 +10833,7 @@
         <v>54</v>
       </c>
       <c r="AB105" s="1" t="s">
-        <v>143</v>
+        <v>311</v>
       </c>
       <c r="AE105" s="2"/>
       <c r="AX105" s="2"/>
@@ -10870,7 +10879,7 @@
         <v>54</v>
       </c>
       <c r="AC106" s="1" t="s">
-        <v>144</v>
+        <v>312</v>
       </c>
       <c r="AE106" s="2"/>
       <c r="AX106" s="2"/>
@@ -10913,10 +10922,10 @@
         <v>54</v>
       </c>
       <c r="AB107" s="1" t="s">
-        <v>143</v>
+        <v>311</v>
       </c>
       <c r="AC107" s="1" t="s">
-        <v>144</v>
+        <v>312</v>
       </c>
       <c r="AE107" s="2"/>
       <c r="AX107" s="2"/>
@@ -10959,7 +10968,7 @@
         <v>107</v>
       </c>
       <c r="AA108" s="1" t="s">
-        <v>141</v>
+        <v>310</v>
       </c>
       <c r="AE108" s="2"/>
       <c r="AX108" s="2"/>
@@ -11002,7 +11011,7 @@
         <v>107</v>
       </c>
       <c r="AB109" s="1" t="s">
-        <v>143</v>
+        <v>311</v>
       </c>
       <c r="AE109" s="2"/>
       <c r="AX109" s="2"/>
@@ -11048,7 +11057,7 @@
         <v>107</v>
       </c>
       <c r="AC110" s="1" t="s">
-        <v>144</v>
+        <v>312</v>
       </c>
       <c r="AE110" s="2"/>
       <c r="AX110" s="2"/>
@@ -11091,10 +11100,10 @@
         <v>107</v>
       </c>
       <c r="AB111" s="1" t="s">
-        <v>143</v>
+        <v>311</v>
       </c>
       <c r="AC111" s="1" t="s">
-        <v>144</v>
+        <v>312</v>
       </c>
       <c r="AE111" s="2"/>
       <c r="AX111" s="2"/>
@@ -11137,7 +11146,7 @@
         <v>119</v>
       </c>
       <c r="AA112" s="1" t="s">
-        <v>141</v>
+        <v>310</v>
       </c>
       <c r="AE112" s="2"/>
       <c r="AX112" s="2"/>
@@ -11180,7 +11189,7 @@
         <v>119</v>
       </c>
       <c r="AB113" s="1" t="s">
-        <v>143</v>
+        <v>311</v>
       </c>
       <c r="AE113" s="2"/>
       <c r="AX113" s="2"/>
@@ -11226,7 +11235,7 @@
         <v>119</v>
       </c>
       <c r="AC114" s="1" t="s">
-        <v>144</v>
+        <v>312</v>
       </c>
       <c r="AE114" s="2"/>
       <c r="AX114" s="2"/>
@@ -11269,10 +11278,10 @@
         <v>119</v>
       </c>
       <c r="AB115" s="1" t="s">
-        <v>143</v>
+        <v>311</v>
       </c>
       <c r="AC115" s="1" t="s">
-        <v>144</v>
+        <v>312</v>
       </c>
       <c r="AE115" s="2"/>
       <c r="AX115" s="2"/>

</xml_diff>